<commit_message>
added Tag Controller Integration tests
</commit_message>
<xml_diff>
--- a/EverNoteApi_map.xlsx
+++ b/EverNoteApi_map.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>URL Path</t>
   </si>
@@ -40,43 +40,58 @@
     <t>Get all the persons</t>
   </si>
   <si>
-    <t>Get all the notepads for a person with the specified id</t>
-  </si>
-  <si>
-    <t>/person/{id}/pad/{name}</t>
-  </si>
-  <si>
-    <t>Get all the tags for a user with the specified id</t>
-  </si>
-  <si>
-    <t>Get, create, update or delete single note for a user with the specified id</t>
-  </si>
-  <si>
-    <t>Get, create, update or delete single pad by the specified Name</t>
-  </si>
-  <si>
-    <t>/person/{id}/pad/{padName}/note/{noteId}</t>
-  </si>
-  <si>
     <t>/person/{id}/tag/{tagName}</t>
   </si>
   <si>
-    <t>Get, create, update or delete single note by the specified noteId, padName and userId</t>
-  </si>
-  <si>
-    <t>Get all the notes from a pad with the specified padName and userId</t>
-  </si>
-  <si>
     <t>/person</t>
   </si>
   <si>
     <t>/person/{id}/pad</t>
   </si>
   <si>
-    <t>/person/{id}/pad/{padName}/note</t>
-  </si>
-  <si>
     <t>/person/{id}/tag</t>
+  </si>
+  <si>
+    <t>/person/{id}/pad/{padId}</t>
+  </si>
+  <si>
+    <t>/person/{id}/pad/{padId}/note</t>
+  </si>
+  <si>
+    <t>/person/{id}/pad/{padId}/note/{noteId}</t>
+  </si>
+  <si>
+    <t>POST,DELETE</t>
+  </si>
+  <si>
+    <t>/person/{id}/pad/{padId}/note/{noteId}/tag</t>
+  </si>
+  <si>
+    <t>/person/{id}/pad/{padId}/note/{noteId}/tag/{tagName}</t>
+  </si>
+  <si>
+    <t>Create or delete single tag for a note</t>
+  </si>
+  <si>
+    <t>Get all the tags for a note</t>
+  </si>
+  <si>
+    <t>Get all the tags for a person</t>
+  </si>
+  <si>
+    <t>Get all the tags with name {tagName} for a person</t>
+  </si>
+  <si>
+    <t>Get, create, update or delete single note</t>
+  </si>
+  <si>
+    <t>Get all the notes for a pad</t>
+  </si>
+  <si>
+    <t>Get, create, update or delete single pad</t>
+  </si>
+  <si>
+    <t>Get all the notepads for a person</t>
   </si>
 </sst>
 </file>
@@ -120,11 +135,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -433,7 +449,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +472,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -478,76 +494,97 @@
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="2" t="s">
+    </row>
+    <row r="16" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>11</v>
+      <c r="C16" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
REST is now with "/api"-prefix
</commit_message>
<xml_diff>
--- a/EverNoteApi_map.xlsx
+++ b/EverNoteApi_map.xlsx
@@ -34,42 +34,12 @@
     <t>Get, create, update or delete single person by the specified id</t>
   </si>
   <si>
-    <t>/person/{id}</t>
-  </si>
-  <si>
     <t>Get all the persons</t>
   </si>
   <si>
-    <t>/person/{id}/tag/{tagName}</t>
-  </si>
-  <si>
-    <t>/person</t>
-  </si>
-  <si>
-    <t>/person/{id}/pad</t>
-  </si>
-  <si>
-    <t>/person/{id}/tag</t>
-  </si>
-  <si>
-    <t>/person/{id}/pad/{padId}</t>
-  </si>
-  <si>
-    <t>/person/{id}/pad/{padId}/note</t>
-  </si>
-  <si>
-    <t>/person/{id}/pad/{padId}/note/{noteId}</t>
-  </si>
-  <si>
     <t>POST,DELETE</t>
   </si>
   <si>
-    <t>/person/{id}/pad/{padId}/note/{noteId}/tag</t>
-  </si>
-  <si>
-    <t>/person/{id}/pad/{padId}/note/{noteId}/tag/{tagName}</t>
-  </si>
-  <si>
     <t>Create or delete single tag for a note</t>
   </si>
   <si>
@@ -92,6 +62,36 @@
   </si>
   <si>
     <t>Get all the notepads for a person</t>
+  </si>
+  <si>
+    <t>/api/person</t>
+  </si>
+  <si>
+    <t>/api/person/{id}</t>
+  </si>
+  <si>
+    <t>/api/person/{id}/pad</t>
+  </si>
+  <si>
+    <t>/api/person/{id}/pad/{padId}</t>
+  </si>
+  <si>
+    <t>/api/person/{id}/pad/{padId}/note</t>
+  </si>
+  <si>
+    <t>/api/person/{id}/pad/{padId}/note/{noteId}</t>
+  </si>
+  <si>
+    <t>/api/person/{id}/pad/{padId}/note/{noteId}/tag</t>
+  </si>
+  <si>
+    <t>/api/person/{id}/pad/{padId}/note/{noteId}/tag/{tagName}</t>
+  </si>
+  <si>
+    <t>/api/person/{id}/tag</t>
+  </si>
+  <si>
+    <t>/api/person/{id}/tag/{tagName}</t>
   </si>
 </sst>
 </file>
@@ -472,18 +472,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -494,91 +494,91 @@
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>